<commit_message>
V9, uses neshawk, with better emulation, 74 frames faster
</commit_message>
<xml_diff>
--- a/BattleChess/FrameCompare.xlsx
+++ b/BattleChess/FrameCompare.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\BattleChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB79BD5-0C5F-44C9-91F0-BE976193DDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FBA502-D366-46B8-A738-F991F9FBAC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="4410" windowWidth="15375" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37365" yWindow="1410" windowWidth="15375" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="V4" sheetId="9" r:id="rId1"/>
-    <sheet name="V3" sheetId="8" r:id="rId2"/>
+    <sheet name="V9" sheetId="10" r:id="rId1"/>
+    <sheet name="V8" sheetId="8" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>Place</t>
   </si>
@@ -39,78 +39,12 @@
     <t>diff</t>
   </si>
   <si>
-    <t>V3</t>
-  </si>
-  <si>
-    <t>Area 1 appears</t>
-  </si>
-  <si>
-    <t>Area 2 appears</t>
-  </si>
-  <si>
-    <t>Area 3 appears</t>
-  </si>
-  <si>
-    <t>Area 4 appears</t>
-  </si>
-  <si>
-    <t>Boss 1 flash</t>
-  </si>
-  <si>
-    <t>1st Hit</t>
-  </si>
-  <si>
-    <t>Boss 2 flah</t>
-  </si>
-  <si>
-    <t>Start warp</t>
-  </si>
-  <si>
-    <t>Boss 2 flash</t>
-  </si>
-  <si>
-    <t>1st Move</t>
-  </si>
-  <si>
-    <t>Boss 3 flash</t>
-  </si>
-  <si>
-    <t>Area 5 appears</t>
-  </si>
-  <si>
-    <t>Area 6 appears</t>
-  </si>
-  <si>
-    <t>Area 7 appears</t>
-  </si>
-  <si>
-    <t>Area 9 appears</t>
-  </si>
-  <si>
-    <t>Boss 4 flash</t>
-  </si>
-  <si>
-    <t>Area 10 appears</t>
-  </si>
-  <si>
-    <t>Final Boss flash</t>
-  </si>
-  <si>
-    <t>Area 11 appears</t>
-  </si>
-  <si>
-    <t>Area 12 appears</t>
-  </si>
-  <si>
     <t>END</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>V4</t>
-  </si>
-  <si>
     <t>V8</t>
   </si>
   <si>
@@ -184,6 +118,18 @@
   </si>
   <si>
     <t>screen appears (take back 4)</t>
+  </si>
+  <si>
+    <t>Menu starts</t>
+  </si>
+  <si>
+    <t>black screen (take back 2)</t>
+  </si>
+  <si>
+    <t>black screen (take back 3)</t>
+  </si>
+  <si>
+    <t>V9</t>
   </si>
 </sst>
 </file>
@@ -193,26 +139,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -314,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -322,52 +254,35 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -687,1601 +602,1286 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092D6BE4-4D06-4643-B3BA-0E1A41EB7467}">
-  <dimension ref="A1:F226"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2B1C4D-EE3C-47DC-9064-22D3CE5B342A}">
+  <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="8.75" customWidth="1"/>
     <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2">
+        <v>60</v>
+      </c>
+      <c r="D2" s="3">
+        <f t="shared" ref="D2:D29" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <v>10</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>158</v>
+      </c>
+      <c r="C3" s="2">
+        <v>168</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>257</v>
+      </c>
+      <c r="C4" s="2">
+        <v>289</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>285</v>
+      </c>
+      <c r="C5" s="2">
+        <v>317</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>339</v>
+      </c>
+      <c r="C6" s="2">
+        <v>382</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2">
+        <v>345</v>
+      </c>
+      <c r="C7" s="2">
+        <v>388</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>402</v>
+      </c>
+      <c r="C8" s="2">
+        <v>445</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>563</v>
+      </c>
+      <c r="C9" s="2">
+        <v>605</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1043</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1085</v>
+      </c>
+      <c r="D10" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4187</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4229</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E11" s="12">
+        <f>B11-B10</f>
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="7">
+        <v>5324</v>
+      </c>
+      <c r="C12" s="7">
+        <v>5366</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="7">
+        <v>16782</v>
+      </c>
+      <c r="C13" s="7">
+        <v>16824</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E13" s="11">
+        <f>B13-B12</f>
+        <v>11458</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="7">
+        <v>18979</v>
+      </c>
+      <c r="C14" s="7">
+        <v>19021</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <v>24523</v>
+      </c>
+      <c r="C15" s="2">
+        <v>24565</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E15" s="12">
+        <f>B15-B14</f>
+        <v>5544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2">
+        <v>28558</v>
+      </c>
+      <c r="C16" s="2">
+        <v>28600</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <v>29860</v>
+      </c>
+      <c r="C17" s="2">
+        <v>29902</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E17" s="12">
+        <f>B17-B16</f>
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
+        <v>31357</v>
+      </c>
+      <c r="C18" s="2">
+        <v>31398</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2">
+        <v>36501</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E19" s="12">
+        <f>B19-B18</f>
+        <v>-31357</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
+        <v>37650</v>
+      </c>
+      <c r="C20" s="2">
+        <v>37691</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2">
+        <v>37662</v>
+      </c>
+      <c r="C21" s="2">
+        <v>37703</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2">
+        <v>37914</v>
+      </c>
+      <c r="C22" s="2">
+        <v>37959</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2">
+        <v>37956</v>
+      </c>
+      <c r="C23" s="2">
+        <v>38001</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2">
+        <v>38207</v>
+      </c>
+      <c r="C24" s="2">
+        <v>38266</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="2">
+        <v>39557</v>
+      </c>
+      <c r="C25" s="2">
+        <v>39616</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="E25" s="12">
+        <f>B25-B24</f>
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2">
+        <v>40779</v>
+      </c>
+      <c r="C26" s="2">
+        <v>40837</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>41032</v>
+      </c>
+      <c r="C27" s="2">
+        <v>41100</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>41314</v>
+      </c>
+      <c r="C28" s="2">
+        <v>41388</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="4">
+        <v>41344</v>
+      </c>
+      <c r="C29" s="4">
+        <v>41418</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="E29" s="4">
+        <v>41303</v>
+      </c>
+      <c r="F29" s="3">
+        <f>E29-B29</f>
+        <v>-41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>100</v>
-      </c>
-      <c r="C2" s="2">
-        <v>100</v>
-      </c>
-      <c r="D2" s="3">
-        <f t="shared" ref="D2:D55" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>3519</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3519</v>
-      </c>
-      <c r="D3" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3529</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3529</v>
-      </c>
-      <c r="D4" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>5901</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5901</v>
-      </c>
-      <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5931</v>
-      </c>
-      <c r="C6" s="2">
-        <v>5931</v>
-      </c>
-      <c r="D6" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6">
-        <v>10562</v>
-      </c>
-      <c r="C7" s="6">
-        <v>10562</v>
-      </c>
-      <c r="D7" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2">
-        <v>10913</v>
-      </c>
-      <c r="C8" s="2">
-        <v>10913</v>
-      </c>
-      <c r="D8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6">
-        <v>18026</v>
-      </c>
-      <c r="C9" s="6">
-        <v>18026</v>
-      </c>
-      <c r="D9" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2">
-        <v>18377</v>
-      </c>
-      <c r="C10" s="2">
-        <v>18377</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2">
-        <v>20284</v>
-      </c>
-      <c r="C11" s="2">
-        <v>20284</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2">
-        <v>20324</v>
-      </c>
-      <c r="C12" s="2">
-        <v>20324</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="2">
-        <v>28497</v>
-      </c>
-      <c r="C13" s="2">
-        <v>28497</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2">
-        <v>28537</v>
-      </c>
-      <c r="C14" s="2">
-        <v>28537</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2">
-        <v>28830</v>
-      </c>
-      <c r="C15" s="2">
-        <v>28830</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="2">
-        <v>30560</v>
-      </c>
-      <c r="C16" s="2">
-        <v>30560</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="10">
-        <v>31598</v>
-      </c>
-      <c r="C17" s="10">
-        <v>31598</v>
-      </c>
-      <c r="D17" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2">
-        <v>31949</v>
-      </c>
-      <c r="C18" s="2">
-        <v>31949</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="2">
-        <v>35453</v>
-      </c>
-      <c r="C19" s="2">
-        <v>35453</v>
-      </c>
-      <c r="D19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>35447</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="2">
-        <v>35587</v>
-      </c>
-      <c r="C20" s="2">
-        <v>35587</v>
-      </c>
-      <c r="D20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="2">
-        <v>37987</v>
-      </c>
-      <c r="C21" s="2">
-        <v>37987</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="2">
-        <v>38007</v>
-      </c>
-      <c r="C22" s="2">
-        <v>38007</v>
-      </c>
-      <c r="D22" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="6">
-        <v>44428</v>
-      </c>
-      <c r="C23" s="6">
-        <v>44428</v>
-      </c>
-      <c r="D23" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="2">
-        <v>45744</v>
-      </c>
-      <c r="C24" s="2">
-        <v>45744</v>
-      </c>
-      <c r="D24" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="6">
-        <v>52410</v>
-      </c>
-      <c r="C25" s="6">
-        <v>52410</v>
-      </c>
-      <c r="D25" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="2">
-        <v>52762</v>
-      </c>
-      <c r="C26" s="2">
-        <v>52762</v>
-      </c>
-      <c r="D26" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="2">
-        <v>57870</v>
-      </c>
-      <c r="C27" s="2">
-        <v>57870</v>
-      </c>
-      <c r="D27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="6">
-        <v>65702</v>
-      </c>
-      <c r="C28" s="6">
-        <v>65702</v>
-      </c>
-      <c r="D28" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="8">
-        <v>67016</v>
-      </c>
-      <c r="C29" s="8">
-        <v>67016</v>
-      </c>
-      <c r="D29" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="6">
-        <v>73197</v>
-      </c>
-      <c r="C30" s="6">
-        <v>73197</v>
-      </c>
-      <c r="D30" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="2">
-        <v>73549</v>
-      </c>
-      <c r="C31" s="2">
-        <v>73549</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="2">
-        <v>75730</v>
-      </c>
-      <c r="C32" s="2">
-        <v>75730</v>
-      </c>
-      <c r="D32" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="2">
-        <v>75839</v>
-      </c>
-      <c r="C33" s="2">
-        <v>75839</v>
-      </c>
-      <c r="D33" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="2">
-        <v>78321</v>
-      </c>
-      <c r="C35" s="2">
-        <v>78321</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="2">
-        <v>79677</v>
-      </c>
-      <c r="C36" s="2">
-        <v>79677</v>
-      </c>
-      <c r="D36" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="2">
-        <v>79726</v>
-      </c>
-      <c r="C37" s="2">
-        <v>79726</v>
-      </c>
-      <c r="D37" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="2">
-        <v>82654</v>
-      </c>
-      <c r="C39" s="2">
-        <v>82654</v>
-      </c>
-      <c r="D39" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" s="6">
-        <v>85080</v>
-      </c>
-      <c r="C41" s="6">
-        <v>85080</v>
-      </c>
-      <c r="D41" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="2">
-        <v>86397</v>
-      </c>
-      <c r="C42" s="2">
-        <v>86397</v>
-      </c>
-      <c r="D42" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43" s="2">
-        <v>87256</v>
-      </c>
-      <c r="C43" s="2">
-        <v>87256</v>
-      </c>
-      <c r="D43" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="2">
-        <v>87296</v>
-      </c>
-      <c r="C44" s="2">
-        <v>87296</v>
-      </c>
-      <c r="D44" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="2">
-        <v>87687</v>
-      </c>
-      <c r="C45" s="2">
-        <v>87687</v>
-      </c>
+      <c r="C30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="3"/>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="3"/>
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="3"/>
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="3"/>
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="3"/>
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="3"/>
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="3"/>
+      <c r="F42"/>
+    </row>
+    <row r="43" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="3"/>
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="3"/>
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
       <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" s="2">
-        <v>92069</v>
-      </c>
-      <c r="C47" s="2">
-        <v>92069</v>
-      </c>
-      <c r="D47" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" s="2">
-        <v>97334</v>
-      </c>
-      <c r="C48" s="2">
-        <v>97334</v>
-      </c>
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="3"/>
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="3"/>
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
       <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="4">
-        <v>97414</v>
-      </c>
-      <c r="C49" s="4">
-        <v>97414</v>
-      </c>
-      <c r="D49" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B50" s="14">
-        <v>100685</v>
-      </c>
-      <c r="C50" s="14">
-        <v>100685</v>
-      </c>
-      <c r="D50" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B51" s="4">
-        <v>102001</v>
-      </c>
-      <c r="C51" s="4">
-        <v>102001</v>
-      </c>
-      <c r="D51" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" s="4">
-        <v>120608</v>
-      </c>
-      <c r="C52" s="4">
-        <v>120608</v>
-      </c>
-      <c r="D52" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B53" s="14">
-        <v>121088</v>
-      </c>
-      <c r="C53" s="14">
-        <v>121103</v>
-      </c>
-      <c r="D53" s="7">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E53" s="14"/>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B54" s="4">
-        <v>122403</v>
-      </c>
-      <c r="C54" s="4">
-        <v>122418</v>
-      </c>
-      <c r="D54" s="3">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E54" s="4"/>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B55" s="4">
-        <v>122661</v>
-      </c>
-      <c r="C55" s="4">
-        <v>122676</v>
-      </c>
-      <c r="D55" s="3">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="3"/>
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="3"/>
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="3"/>
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="3"/>
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="3"/>
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="3"/>
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="3"/>
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
       <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="3"/>
-    </row>
-    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="3"/>
-    </row>
-    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
-      <c r="D62" s="3"/>
-    </row>
-    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D62"/>
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
+      <c r="D63"/>
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
-      <c r="D64" s="3"/>
-    </row>
-    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
+      <c r="D64"/>
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
+      <c r="D65"/>
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
+      <c r="D66"/>
+      <c r="F66"/>
+    </row>
+    <row r="67" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
+      <c r="D67"/>
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
-      <c r="D68" s="3"/>
-    </row>
-    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
-      <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
-      <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
-      <c r="D72" s="3"/>
-    </row>
-    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
-      <c r="D73" s="3"/>
-    </row>
-    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
-      <c r="D74" s="3"/>
-    </row>
-    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
-      <c r="D75" s="3"/>
-    </row>
-    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
-      <c r="D76" s="3"/>
-    </row>
-    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
-      <c r="D77" s="3"/>
-    </row>
-    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
-      <c r="D78" s="3"/>
-    </row>
-    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
-      <c r="D79" s="3"/>
-    </row>
-    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
-      <c r="D80" s="3"/>
-    </row>
-    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
-      <c r="D81" s="3"/>
-    </row>
-    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
-      <c r="D82" s="3"/>
-    </row>
-    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
-      <c r="D83" s="3"/>
-    </row>
-    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
-      <c r="D84" s="3"/>
-    </row>
-    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
-      <c r="D85" s="3"/>
-    </row>
-    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
-      <c r="D86" s="3"/>
-    </row>
-    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
-      <c r="D87" s="3"/>
-    </row>
-    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
     </row>
-    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
     </row>
-    <row r="97" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
     </row>
-    <row r="98" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
     </row>
-    <row r="100" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
     </row>
-    <row r="102" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
     </row>
-    <row r="103" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
     </row>
-    <row r="104" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
     </row>
-    <row r="105" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
     </row>
-    <row r="109" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
     </row>
-    <row r="110" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
     </row>
-    <row r="111" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
     </row>
-    <row r="112" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
     </row>
-    <row r="113" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
     </row>
-    <row r="114" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
     </row>
-    <row r="115" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
     </row>
-    <row r="117" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
     </row>
-    <row r="118" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
     </row>
-    <row r="119" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
     </row>
-    <row r="120" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
     </row>
-    <row r="121" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
     </row>
-    <row r="122" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
     </row>
-    <row r="123" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
     </row>
-    <row r="124" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
     </row>
-    <row r="125" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
     </row>
-    <row r="126" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
     </row>
-    <row r="127" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
     </row>
-    <row r="128" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
     </row>
-    <row r="129" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
     </row>
-    <row r="130" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
     </row>
-    <row r="131" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
     </row>
-    <row r="132" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
     </row>
-    <row r="133" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
     </row>
-    <row r="134" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
     </row>
-    <row r="135" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
     </row>
-    <row r="136" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
     </row>
-    <row r="137" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
     </row>
-    <row r="138" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
     </row>
-    <row r="139" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
     </row>
-    <row r="140" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
     </row>
-    <row r="141" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
     </row>
-    <row r="142" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
     </row>
-    <row r="143" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
     </row>
-    <row r="144" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
     </row>
-    <row r="145" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
     </row>
-    <row r="146" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
     </row>
-    <row r="147" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
     </row>
-    <row r="148" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
     </row>
-    <row r="149" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
     </row>
-    <row r="150" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
     </row>
-    <row r="151" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
     </row>
-    <row r="152" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
     </row>
-    <row r="153" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
     </row>
-    <row r="154" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
     </row>
-    <row r="155" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
     </row>
-    <row r="156" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
     </row>
-    <row r="157" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
     </row>
-    <row r="158" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
     </row>
-    <row r="159" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
     </row>
-    <row r="160" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
     </row>
-    <row r="161" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
     </row>
-    <row r="162" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
     </row>
-    <row r="163" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
     </row>
-    <row r="164" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
     </row>
-    <row r="165" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
     </row>
-    <row r="166" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
     </row>
-    <row r="167" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
     </row>
-    <row r="168" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
     </row>
-    <row r="169" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
     </row>
-    <row r="170" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
     </row>
-    <row r="171" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
     </row>
-    <row r="172" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
     </row>
-    <row r="173" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
     </row>
-    <row r="174" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
     </row>
-    <row r="175" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
     </row>
-    <row r="176" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
     </row>
-    <row r="177" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
     </row>
-    <row r="178" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
     </row>
-    <row r="179" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
     </row>
-    <row r="180" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
     </row>
-    <row r="181" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
     </row>
-    <row r="182" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
     </row>
-    <row r="183" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
     </row>
-    <row r="184" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
     </row>
-    <row r="185" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
     </row>
-    <row r="186" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
     </row>
-    <row r="187" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
     </row>
-    <row r="188" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
     </row>
-    <row r="189" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
     </row>
-    <row r="190" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
     </row>
-    <row r="191" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
     </row>
-    <row r="192" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
     </row>
-    <row r="193" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" s="4"/>
       <c r="C193" s="4"/>
     </row>
-    <row r="194" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" s="4"/>
       <c r="C194" s="4"/>
     </row>
-    <row r="195" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" s="4"/>
       <c r="C195" s="4"/>
     </row>
-    <row r="196" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" s="4"/>
       <c r="C196" s="4"/>
     </row>
-    <row r="197" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" s="4"/>
       <c r="C197" s="4"/>
     </row>
-    <row r="198" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" s="4"/>
       <c r="C198" s="4"/>
     </row>
-    <row r="199" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" s="4"/>
       <c r="C199" s="4"/>
     </row>
-    <row r="200" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" s="4"/>
       <c r="C200" s="4"/>
-    </row>
-    <row r="201" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B201" s="4"/>
-      <c r="C201" s="4"/>
-    </row>
-    <row r="202" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B202" s="4"/>
-      <c r="C202" s="4"/>
-    </row>
-    <row r="203" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B203" s="4"/>
-      <c r="C203" s="4"/>
-    </row>
-    <row r="204" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B204" s="4"/>
-      <c r="C204" s="4"/>
-    </row>
-    <row r="205" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B205" s="4"/>
-      <c r="C205" s="4"/>
-    </row>
-    <row r="206" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B206" s="4"/>
-      <c r="C206" s="4"/>
-    </row>
-    <row r="207" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B207" s="4"/>
-      <c r="C207" s="4"/>
-    </row>
-    <row r="208" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B208" s="4"/>
-      <c r="C208" s="4"/>
-    </row>
-    <row r="209" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B209" s="4"/>
-      <c r="C209" s="4"/>
-    </row>
-    <row r="210" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B210" s="4"/>
-      <c r="C210" s="4"/>
-    </row>
-    <row r="211" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B211" s="4"/>
-      <c r="C211" s="4"/>
-    </row>
-    <row r="212" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B212" s="4"/>
-      <c r="C212" s="4"/>
-    </row>
-    <row r="213" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B213" s="4"/>
-      <c r="C213" s="4"/>
-    </row>
-    <row r="214" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B214" s="4"/>
-      <c r="C214" s="4"/>
-    </row>
-    <row r="215" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B215" s="4"/>
-      <c r="C215" s="4"/>
-    </row>
-    <row r="216" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B216" s="4"/>
-      <c r="C216" s="4"/>
-    </row>
-    <row r="217" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B217" s="4"/>
-      <c r="C217" s="4"/>
-    </row>
-    <row r="218" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B218" s="4"/>
-      <c r="C218" s="4"/>
-    </row>
-    <row r="219" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B219" s="4"/>
-      <c r="C219" s="4"/>
-    </row>
-    <row r="220" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B220" s="4"/>
-      <c r="C220" s="4"/>
-    </row>
-    <row r="221" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B221" s="4"/>
-      <c r="C221" s="4"/>
-    </row>
-    <row r="222" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B222" s="4"/>
-      <c r="C222" s="4"/>
-    </row>
-    <row r="223" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B223" s="4"/>
-      <c r="C223" s="4"/>
-    </row>
-    <row r="224" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B224" s="4"/>
-      <c r="C224" s="4"/>
-    </row>
-    <row r="225" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B225" s="4"/>
-      <c r="C225" s="4"/>
-    </row>
-    <row r="226" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B226" s="4"/>
-      <c r="C226" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2293,9 +1893,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F75CE0-A1C1-4DE3-8C32-09CA7DE610E7}">
   <dimension ref="A1:F197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2303,7 +1903,7 @@
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="8.75" customWidth="1"/>
     <col min="4" max="4" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="9" style="18"/>
+    <col min="5" max="5" width="9" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2311,18 +1911,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>28</v>
+      <c r="A2" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>60</v>
@@ -2337,8 +1937,8 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>30</v>
+      <c r="A3" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>168</v>
@@ -2350,8 +1950,8 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>29</v>
+      <c r="A4" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <v>289</v>
@@ -2366,8 +1966,8 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>32</v>
+      <c r="A5" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>317</v>
@@ -2382,8 +1982,8 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>31</v>
+      <c r="A6" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="B6" s="2">
         <v>382</v>
@@ -2397,8 +1997,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>33</v>
+      <c r="A7" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>457</v>
@@ -2412,8 +2012,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>34</v>
+      <c r="A8" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>605</v>
@@ -2427,87 +2027,92 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="15">
+      <c r="A9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="6">
         <v>1085</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="7">
         <v>1042</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="8">
         <f t="shared" ref="D9:D26" si="1">IF(C9&lt;&gt;"",IF(B9&lt;&gt;"",C9-B9,"-"), "-")</f>
         <v>-43</v>
       </c>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="16">
+      <c r="A10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="7">
         <v>4229</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="7">
         <v>4186</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="8">
         <f t="shared" si="1"/>
         <v>-43</v>
       </c>
+      <c r="E10" s="12">
+        <f>B10-B9</f>
+        <v>3144</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="16">
+      <c r="A11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="7">
         <v>5366</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="7">
         <v>5323</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="8">
         <f t="shared" si="1"/>
         <v>-43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="16">
+      <c r="A12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="7">
         <v>16824</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="7">
         <v>16781</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="8">
         <f t="shared" si="1"/>
         <v>-43</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="11">
         <f>B12-B11</f>
         <v>11458</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="16">
+      <c r="A13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="7">
         <v>19021</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="7">
         <v>18978</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="8">
         <f t="shared" si="1"/>
         <v>-43</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>40</v>
+      <c r="A14" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="B14" s="2">
         <v>24565</v>
@@ -2519,14 +2124,14 @@
         <f t="shared" si="1"/>
         <v>-43</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="12">
         <f>B14-B13</f>
         <v>5544</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>41</v>
+      <c r="A15" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="B15" s="2">
         <v>28600</v>
@@ -2540,8 +2145,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>42</v>
+      <c r="A16" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="B16" s="2">
         <v>29902</v>
@@ -2553,10 +2158,14 @@
         <f t="shared" si="1"/>
         <v>-47</v>
       </c>
+      <c r="E16" s="12">
+        <f>B16-B15</f>
+        <v>1302</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>43</v>
+      <c r="A17" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="B17" s="2">
         <v>31398</v>
@@ -2570,8 +2179,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>44</v>
+      <c r="A18" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="B18" s="2">
         <v>36501</v>
@@ -2583,10 +2192,14 @@
         <f t="shared" si="1"/>
         <v>-47</v>
       </c>
+      <c r="E18" s="12">
+        <f>B18-B17</f>
+        <v>5103</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>45</v>
+      <c r="A19" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="B19" s="2">
         <v>37691</v>
@@ -2600,8 +2213,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>47</v>
+      <c r="A20" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="B20" s="2">
         <v>37703</v>
@@ -2615,8 +2228,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>46</v>
+      <c r="A21" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="B21" s="2">
         <v>37959</v>
@@ -2630,8 +2243,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>48</v>
+      <c r="A22" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="B22" s="2">
         <v>38266</v>
@@ -2645,8 +2258,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>42</v>
+      <c r="A23" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="B23" s="2">
         <v>39616</v>
@@ -2658,10 +2271,14 @@
         <f t="shared" si="1"/>
         <v>-93</v>
       </c>
+      <c r="E23" s="12">
+        <f>B23-B22</f>
+        <v>1350</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>49</v>
+      <c r="A24" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="B24" s="2">
         <v>41100</v>
@@ -2675,8 +2292,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>50</v>
+      <c r="A25" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="B25" s="2">
         <v>41388</v>
@@ -2690,8 +2307,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>23</v>
+      <c r="A26" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="B26" s="4">
         <v>41418</v>
@@ -2713,8 +2330,8 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="12" t="s">
-        <v>24</v>
+      <c r="B27" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="3"/>

</xml_diff>

<commit_message>
v10 - 27 frames faster by delaying to get the cpu to move slightly sooner
</commit_message>
<xml_diff>
--- a/BattleChess/FrameCompare.xlsx
+++ b/BattleChess/FrameCompare.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\BattleChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FBA502-D366-46B8-A738-F991F9FBAC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EA4C37-31E8-4E30-9BB3-549664394196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37365" yWindow="1410" windowWidth="15375" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="7305" windowWidth="15375" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="V9" sheetId="10" r:id="rId1"/>
-    <sheet name="V8" sheetId="8" r:id="rId2"/>
+    <sheet name="V10" sheetId="11" r:id="rId1"/>
+    <sheet name="V9" sheetId="10" r:id="rId2"/>
+    <sheet name="V8" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="49">
   <si>
     <t>Place</t>
   </si>
@@ -130,6 +131,54 @@
   </si>
   <si>
     <t>V9</t>
+  </si>
+  <si>
+    <t>V10</t>
+  </si>
+  <si>
+    <t>Menu appears</t>
+  </si>
+  <si>
+    <t>Black screen</t>
+  </si>
+  <si>
+    <t>Fight animation ends (black screen)</t>
+  </si>
+  <si>
+    <t>Knight highlighted</t>
+  </si>
+  <si>
+    <t>Bishop highlighted</t>
+  </si>
+  <si>
+    <t>King highlighted</t>
+  </si>
+  <si>
+    <t>Pawn highlighted</t>
+  </si>
+  <si>
+    <t>Pawn move start</t>
+  </si>
+  <si>
+    <t>Cpu think time</t>
+  </si>
+  <si>
+    <t>Dropdown starts</t>
+  </si>
+  <si>
+    <t>Blackscreen</t>
+  </si>
+  <si>
+    <t>blackscreen (menu start for takeback 2)</t>
+  </si>
+  <si>
+    <t>black screen (fight start)</t>
+  </si>
+  <si>
+    <t>black screen (fight end)</t>
+  </si>
+  <si>
+    <t>black screen (end menu)</t>
   </si>
 </sst>
 </file>
@@ -602,12 +651,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2B1C4D-EE3C-47DC-9064-22D3CE5B342A}">
-  <dimension ref="A1:F200"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9413D97-4714-4BE6-950A-23095ABB9287}">
+  <dimension ref="A1:F220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,13 +672,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -640,11 +692,11 @@
         <v>50</v>
       </c>
       <c r="C2" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D29" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
-        <v>10</v>
+        <f t="shared" ref="D2:D49" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <v>0</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -656,11 +708,11 @@
         <v>158</v>
       </c>
       <c r="C3" s="2">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D3" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -672,11 +724,11 @@
         <v>257</v>
       </c>
       <c r="C4" s="2">
-        <v>289</v>
+        <v>258</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -688,42 +740,43 @@
         <v>285</v>
       </c>
       <c r="C5" s="2">
-        <v>317</v>
+        <v>286</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2">
+        <v>329</v>
+      </c>
+      <c r="C6" s="2">
+        <v>329</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
         <v>339</v>
       </c>
-      <c r="C6" s="2">
-        <v>382</v>
-      </c>
-      <c r="D6" s="3">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="2">
-        <v>345</v>
-      </c>
       <c r="C7" s="2">
-        <v>388</v>
+        <v>339</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -734,538 +787,712 @@
         <v>402</v>
       </c>
       <c r="C8" s="2">
-        <v>445</v>
+        <v>402</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2">
+        <v>489</v>
+      </c>
+      <c r="C9" s="2">
+        <v>489</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <v>563</v>
       </c>
-      <c r="C9" s="2">
-        <v>605</v>
-      </c>
-      <c r="D9" s="3">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1043</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1085</v>
-      </c>
-      <c r="D10" s="8">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="E10" s="12"/>
+      <c r="C10" s="7">
+        <v>562</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="7">
-        <v>4187</v>
+        <v>13</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1043</v>
       </c>
       <c r="C11" s="7">
-        <v>4229</v>
+        <v>1042</v>
       </c>
       <c r="D11" s="8">
         <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="E11" s="12">
-        <f>B11-B10</f>
-        <v>3144</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="7">
-        <v>5324</v>
+        <v>4187</v>
       </c>
       <c r="C12" s="7">
-        <v>5366</v>
+        <v>4186</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>-1</v>
+      </c>
+      <c r="E12" s="12">
+        <f>B12-B11</f>
+        <v>3144</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="7">
-        <v>16782</v>
+        <v>5324</v>
       </c>
       <c r="C13" s="7">
-        <v>16824</v>
+        <v>5323</v>
       </c>
       <c r="D13" s="8">
         <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="E13" s="11">
-        <f>B13-B12</f>
-        <v>11458</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="7">
+        <v>16782</v>
+      </c>
+      <c r="C14" s="7">
+        <v>16781</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E14" s="11">
+        <f>B14-B13</f>
+        <v>11458</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B15" s="7">
         <v>18979</v>
       </c>
-      <c r="C14" s="7">
-        <v>19021</v>
-      </c>
-      <c r="D14" s="8">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="2">
-        <v>24523</v>
-      </c>
-      <c r="C15" s="2">
-        <v>24565</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="E15" s="12">
-        <f>B15-B14</f>
-        <v>5544</v>
+      <c r="C15" s="7">
+        <v>18978</v>
+      </c>
+      <c r="D15" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2">
+        <v>24523</v>
+      </c>
+      <c r="C16" s="2">
+        <v>24522</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E16" s="12">
+        <f>B16-B15</f>
+        <v>5544</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2">
+        <v>26633</v>
+      </c>
+      <c r="C17" s="2">
+        <v>26632</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2">
+        <v>26736</v>
+      </c>
+      <c r="C18" s="2">
+        <v>26734</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2">
+        <v>26750</v>
+      </c>
+      <c r="C19" s="2">
+        <v>26748</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="2">
+        <v>28444</v>
+      </c>
+      <c r="C20" s="2">
+        <v>28442</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B21" s="2">
         <v>28558</v>
       </c>
-      <c r="C16" s="2">
-        <v>28600</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="C21" s="2">
+        <v>28554</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B22" s="2">
         <v>29860</v>
       </c>
-      <c r="C17" s="2">
-        <v>29902</v>
-      </c>
-      <c r="D17" s="3">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="E17" s="12">
-        <f>B17-B16</f>
+      <c r="C22" s="2">
+        <v>29855</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E22" s="12">
+        <f>B22-B21</f>
         <v>1302</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="2">
+        <v>30971</v>
+      </c>
+      <c r="C23" s="2">
+        <v>30966</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2">
+        <v>31072</v>
+      </c>
+      <c r="C24" s="2">
+        <v>31066</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E24" s="12"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="2">
+        <v>31078</v>
+      </c>
+      <c r="C25" s="2">
+        <v>31072</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E25" s="12"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="2">
+        <v>31090</v>
+      </c>
+      <c r="C26" s="2">
+        <v>31084</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B27" s="2">
         <v>31357</v>
       </c>
-      <c r="C18" s="2">
-        <v>31398</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="0"/>
+      <c r="C27" s="2">
+        <v>31351</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="2">
+        <v>36460</v>
+      </c>
+      <c r="C28" s="2">
+        <v>36454</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E28" s="12">
+        <f>B28-B27</f>
+        <v>5103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="2">
+        <v>37366</v>
+      </c>
+      <c r="C29" s="2">
+        <v>37360</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E29" s="12"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2">
-        <v>36501</v>
-      </c>
-      <c r="D19" s="3" t="str">
+      <c r="B30" s="2">
+        <v>37382</v>
+      </c>
+      <c r="C30" s="2">
+        <v>37376</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E30" s="12"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="2">
+        <v>37650</v>
+      </c>
+      <c r="C31" s="2">
+        <v>37644</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="2">
+        <v>37662</v>
+      </c>
+      <c r="C32" s="2">
+        <v>37664</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E32" s="2">
+        <v>37662</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2">
+        <v>37707</v>
+      </c>
+      <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E19" s="12">
-        <f>B19-B18</f>
-        <v>-31357</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="2">
-        <v>37650</v>
-      </c>
-      <c r="C20" s="2">
-        <v>37691</v>
-      </c>
-      <c r="D20" s="3">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="2">
-        <v>37662</v>
-      </c>
-      <c r="C21" s="2">
-        <v>37703</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="E33" s="2">
+        <v>37708</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2">
+        <v>37719</v>
+      </c>
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E34" s="2">
+        <v>37720</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2">
+        <v>37843</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E35" s="2">
+        <v>37844</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2">
+        <v>37913</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E36" s="2">
         <v>37914</v>
       </c>
-      <c r="C22" s="2">
-        <v>37959</v>
-      </c>
-      <c r="D22" s="3">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2">
+        <v>37955</v>
+      </c>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E37" s="2">
+        <v>37956</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2">
+        <v>37999</v>
+      </c>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E38" s="2">
+        <v>37998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2">
+        <v>38011</v>
+      </c>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E39" s="2">
+        <v>38010</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="2">
-        <v>37956</v>
-      </c>
-      <c r="C23" s="2">
-        <v>38001</v>
-      </c>
-      <c r="D23" s="3">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2">
+        <v>38135</v>
+      </c>
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E40" s="2">
+        <v>38134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2">
         <v>38207</v>
       </c>
-      <c r="C24" s="2">
-        <v>38266</v>
-      </c>
-      <c r="D24" s="3">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E41" s="2">
+        <v>38207</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B42" s="2">
+        <v>39532</v>
+      </c>
+      <c r="C42" s="2">
+        <v>39523</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="E42" s="2">
         <v>39557</v>
       </c>
-      <c r="C25" s="2">
-        <v>39616</v>
-      </c>
-      <c r="D25" s="3">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="E25" s="12">
-        <f>B25-B24</f>
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2">
+        <v>40019</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="2">
+        <v>40642</v>
+      </c>
+      <c r="C44" s="2">
+        <v>40633</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="2">
-        <v>40779</v>
-      </c>
-      <c r="C26" s="2">
-        <v>40837</v>
-      </c>
-      <c r="D26" s="3">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="B45" s="2">
+        <v>40752</v>
+      </c>
+      <c r="C45" s="2">
+        <v>40743</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="E45" s="12"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="2">
+        <v>40932</v>
+      </c>
+      <c r="C46" s="2">
+        <v>40921</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="2">
-        <v>41032</v>
-      </c>
-      <c r="C27" s="2">
-        <v>41100</v>
-      </c>
-      <c r="D27" s="3">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="B47" s="2">
+        <v>41004</v>
+      </c>
+      <c r="C47" s="2">
+        <v>40993</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="2">
-        <v>41314</v>
-      </c>
-      <c r="C28" s="2">
-        <v>41388</v>
-      </c>
-      <c r="D28" s="3">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="B48" s="2">
+        <v>41287</v>
+      </c>
+      <c r="C48" s="4">
+        <v>41273</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="0"/>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="4">
-        <v>41344</v>
-      </c>
-      <c r="C29" s="4">
-        <v>41418</v>
-      </c>
-      <c r="D29" s="3">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="E29" s="4">
+      <c r="B49" s="4">
+        <v>41317</v>
+      </c>
+      <c r="C49" s="4">
         <v>41303</v>
       </c>
-      <c r="F29" s="3">
-        <f>E29-B29</f>
-        <v>-41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3"/>
-      <c r="F36"/>
-    </row>
-    <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="3"/>
-      <c r="F37"/>
-    </row>
-    <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="3"/>
-      <c r="F38"/>
-    </row>
-    <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="3"/>
-      <c r="F39"/>
-    </row>
-    <row r="40" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="3"/>
-      <c r="F40"/>
-    </row>
-    <row r="41" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="3"/>
-      <c r="F41"/>
-    </row>
-    <row r="42" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="3"/>
-      <c r="F42"/>
-    </row>
-    <row r="43" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="3"/>
-      <c r="F43"/>
-    </row>
-    <row r="44" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="3"/>
-      <c r="F44"/>
-    </row>
-    <row r="45" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="3"/>
-      <c r="F45"/>
-    </row>
-    <row r="46" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="3"/>
-      <c r="F46"/>
-    </row>
-    <row r="47" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="3"/>
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="3"/>
-      <c r="F48"/>
-    </row>
-    <row r="49" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="3"/>
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="3">
+        <f t="shared" si="0"/>
+        <v>-14</v>
+      </c>
+      <c r="E49" s="4">
+        <v>41303</v>
+      </c>
+      <c r="F49" s="3">
+        <f>E49-B49</f>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+      <c r="B50" s="5"/>
       <c r="C50" s="4"/>
       <c r="D50" s="3"/>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="3"/>
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="3"/>
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="3"/>
-      <c r="F54"/>
-    </row>
-    <row r="55" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="3"/>
-      <c r="F55"/>
     </row>
     <row r="56" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
@@ -1313,157 +1540,217 @@
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
-      <c r="D62"/>
+      <c r="D62" s="3"/>
       <c r="F62"/>
     </row>
     <row r="63" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
-      <c r="D63"/>
+      <c r="D63" s="3"/>
       <c r="F63"/>
     </row>
     <row r="64" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64"/>
+      <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
-      <c r="D64"/>
+      <c r="D64" s="3"/>
       <c r="F64"/>
     </row>
     <row r="65" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65"/>
+      <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
-      <c r="D65"/>
+      <c r="D65" s="3"/>
       <c r="F65"/>
     </row>
     <row r="66" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66"/>
+      <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="D66"/>
+      <c r="D66" s="3"/>
       <c r="F66"/>
     </row>
     <row r="67" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67"/>
+      <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
-      <c r="D67"/>
+      <c r="D67" s="3"/>
       <c r="F67"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D68" s="3"/>
+      <c r="F68"/>
+    </row>
+    <row r="69" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D69" s="3"/>
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D70" s="3"/>
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D71" s="3"/>
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D72" s="3"/>
+      <c r="F72"/>
+    </row>
+    <row r="73" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D73" s="3"/>
+      <c r="F73"/>
+    </row>
+    <row r="74" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D74" s="3"/>
+      <c r="F74"/>
+    </row>
+    <row r="75" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D75" s="3"/>
+      <c r="F75"/>
+    </row>
+    <row r="76" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D76" s="3"/>
+      <c r="F76"/>
+    </row>
+    <row r="77" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D77" s="3"/>
+      <c r="F77"/>
+    </row>
+    <row r="78" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D78" s="3"/>
+      <c r="F78"/>
+    </row>
+    <row r="79" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D79" s="3"/>
+      <c r="F79"/>
+    </row>
+    <row r="80" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="3"/>
+      <c r="F80"/>
+    </row>
+    <row r="81" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="3"/>
+      <c r="F81"/>
+    </row>
+    <row r="82" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D82"/>
+      <c r="F82"/>
+    </row>
+    <row r="83" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D83"/>
+      <c r="F83"/>
+    </row>
+    <row r="84" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D84"/>
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D85"/>
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D86"/>
+      <c r="F86"/>
+    </row>
+    <row r="87" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D87"/>
+      <c r="F87"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
     </row>
@@ -1882,6 +2169,83 @@
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" s="4"/>
       <c r="C200" s="4"/>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B201" s="4"/>
+      <c r="C201" s="4"/>
+    </row>
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B202" s="4"/>
+      <c r="C202" s="4"/>
+    </row>
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B203" s="4"/>
+      <c r="C203" s="4"/>
+    </row>
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B204" s="4"/>
+      <c r="C204" s="4"/>
+    </row>
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B205" s="4"/>
+      <c r="C205" s="4"/>
+    </row>
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B206" s="4"/>
+      <c r="C206" s="4"/>
+    </row>
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B207" s="4"/>
+      <c r="C207" s="4"/>
+    </row>
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B208" s="4"/>
+      <c r="C208" s="4"/>
+    </row>
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B209" s="4"/>
+      <c r="C209" s="4"/>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B210" s="4"/>
+      <c r="C210" s="4"/>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B211" s="4"/>
+      <c r="C211" s="4"/>
+    </row>
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B212" s="4"/>
+      <c r="C212" s="4"/>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B213" s="4"/>
+      <c r="C213" s="4"/>
+    </row>
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B214" s="4"/>
+      <c r="C214" s="4"/>
+    </row>
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B215" s="4"/>
+      <c r="C215" s="4"/>
+    </row>
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B216" s="4"/>
+      <c r="C216" s="4"/>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B217" s="4"/>
+      <c r="C217" s="4"/>
+    </row>
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B218" s="4"/>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B219" s="4"/>
+    </row>
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B220" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1890,12 +2254,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F75CE0-A1C1-4DE3-8C32-09CA7DE610E7}">
-  <dimension ref="A1:F197"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2B1C4D-EE3C-47DC-9064-22D3CE5B342A}">
+  <dimension ref="A1:F200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1911,6 +2275,1294 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2">
+        <v>60</v>
+      </c>
+      <c r="D2" s="3">
+        <f t="shared" ref="D2:D29" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <v>10</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>158</v>
+      </c>
+      <c r="C3" s="2">
+        <v>168</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>257</v>
+      </c>
+      <c r="C4" s="2">
+        <v>289</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>285</v>
+      </c>
+      <c r="C5" s="2">
+        <v>317</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>339</v>
+      </c>
+      <c r="C6" s="2">
+        <v>382</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2">
+        <v>345</v>
+      </c>
+      <c r="C7" s="2">
+        <v>388</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>402</v>
+      </c>
+      <c r="C8" s="2">
+        <v>445</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>563</v>
+      </c>
+      <c r="C9" s="2">
+        <v>605</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1043</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1085</v>
+      </c>
+      <c r="D10" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4187</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4229</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E11" s="12">
+        <f>B11-B10</f>
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="7">
+        <v>5324</v>
+      </c>
+      <c r="C12" s="7">
+        <v>5366</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="7">
+        <v>16782</v>
+      </c>
+      <c r="C13" s="7">
+        <v>16824</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E13" s="11">
+        <f>B13-B12</f>
+        <v>11458</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="7">
+        <v>18979</v>
+      </c>
+      <c r="C14" s="7">
+        <v>19021</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <v>24523</v>
+      </c>
+      <c r="C15" s="2">
+        <v>24565</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E15" s="12">
+        <f>B15-B14</f>
+        <v>5544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2">
+        <v>28558</v>
+      </c>
+      <c r="C16" s="2">
+        <v>28600</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <v>29860</v>
+      </c>
+      <c r="C17" s="2">
+        <v>29902</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E17" s="12">
+        <f>B17-B16</f>
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
+        <v>31357</v>
+      </c>
+      <c r="C18" s="2">
+        <v>31398</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2">
+        <v>36501</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E19" s="12">
+        <f>B19-B18</f>
+        <v>-31357</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
+        <v>37650</v>
+      </c>
+      <c r="C20" s="2">
+        <v>37691</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2">
+        <v>37662</v>
+      </c>
+      <c r="C21" s="2">
+        <v>37703</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2">
+        <v>37914</v>
+      </c>
+      <c r="C22" s="2">
+        <v>37959</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2">
+        <v>37956</v>
+      </c>
+      <c r="C23" s="2">
+        <v>38001</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2">
+        <v>38207</v>
+      </c>
+      <c r="C24" s="2">
+        <v>38266</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="2">
+        <v>39557</v>
+      </c>
+      <c r="C25" s="2">
+        <v>39616</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="E25" s="12">
+        <f>B25-B24</f>
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2">
+        <v>40779</v>
+      </c>
+      <c r="C26" s="2">
+        <v>40837</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>41032</v>
+      </c>
+      <c r="C27" s="2">
+        <v>41100</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>41314</v>
+      </c>
+      <c r="C28" s="2">
+        <v>41388</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="4">
+        <v>41344</v>
+      </c>
+      <c r="C29" s="4">
+        <v>41418</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="E29" s="4">
+        <v>41303</v>
+      </c>
+      <c r="F29" s="3">
+        <f>E29-B29</f>
+        <v>-41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="3"/>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="3"/>
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="3"/>
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="3"/>
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="3"/>
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="3"/>
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="3"/>
+      <c r="F42"/>
+    </row>
+    <row r="43" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="3"/>
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="3"/>
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="3"/>
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="3"/>
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="3"/>
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="3"/>
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="3"/>
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="3"/>
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="3"/>
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="3"/>
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="3"/>
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="3"/>
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="3"/>
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="3"/>
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="3"/>
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="3"/>
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="3"/>
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="3"/>
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="3"/>
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62"/>
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63"/>
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64"/>
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65"/>
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66"/>
+      <c r="F66"/>
+    </row>
+    <row r="67" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67"/>
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B123" s="4"/>
+      <c r="C123" s="4"/>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B124" s="4"/>
+      <c r="C124" s="4"/>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128" s="4"/>
+      <c r="C128" s="4"/>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" s="4"/>
+      <c r="C129" s="4"/>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130" s="4"/>
+      <c r="C130" s="4"/>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132" s="4"/>
+      <c r="C132" s="4"/>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B133" s="4"/>
+      <c r="C133" s="4"/>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134" s="4"/>
+      <c r="C134" s="4"/>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B135" s="4"/>
+      <c r="C135" s="4"/>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B136" s="4"/>
+      <c r="C136" s="4"/>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B137" s="4"/>
+      <c r="C137" s="4"/>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B138" s="4"/>
+      <c r="C138" s="4"/>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B139" s="4"/>
+      <c r="C139" s="4"/>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B140" s="4"/>
+      <c r="C140" s="4"/>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B141" s="4"/>
+      <c r="C141" s="4"/>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B142" s="4"/>
+      <c r="C142" s="4"/>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B143" s="4"/>
+      <c r="C143" s="4"/>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B144" s="4"/>
+      <c r="C144" s="4"/>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" s="4"/>
+      <c r="C145" s="4"/>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B146" s="4"/>
+      <c r="C146" s="4"/>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B147" s="4"/>
+      <c r="C147" s="4"/>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B148" s="4"/>
+      <c r="C148" s="4"/>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B149" s="4"/>
+      <c r="C149" s="4"/>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B150" s="4"/>
+      <c r="C150" s="4"/>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B153" s="4"/>
+      <c r="C153" s="4"/>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B154" s="4"/>
+      <c r="C154" s="4"/>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B155" s="4"/>
+      <c r="C155" s="4"/>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B157" s="4"/>
+      <c r="C157" s="4"/>
+    </row>
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B158" s="4"/>
+      <c r="C158" s="4"/>
+    </row>
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B159" s="4"/>
+      <c r="C159" s="4"/>
+    </row>
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B160" s="4"/>
+      <c r="C160" s="4"/>
+    </row>
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+    </row>
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B162" s="4"/>
+      <c r="C162" s="4"/>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B164" s="4"/>
+      <c r="C164" s="4"/>
+    </row>
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B165" s="4"/>
+      <c r="C165" s="4"/>
+    </row>
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B166" s="4"/>
+      <c r="C166" s="4"/>
+    </row>
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B167" s="4"/>
+      <c r="C167" s="4"/>
+    </row>
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B168" s="4"/>
+      <c r="C168" s="4"/>
+    </row>
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B169" s="4"/>
+      <c r="C169" s="4"/>
+    </row>
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B170" s="4"/>
+      <c r="C170" s="4"/>
+    </row>
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B171" s="4"/>
+      <c r="C171" s="4"/>
+    </row>
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B172" s="4"/>
+      <c r="C172" s="4"/>
+    </row>
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B173" s="4"/>
+      <c r="C173" s="4"/>
+    </row>
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B174" s="4"/>
+      <c r="C174" s="4"/>
+    </row>
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B175" s="4"/>
+      <c r="C175" s="4"/>
+    </row>
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B176" s="4"/>
+      <c r="C176" s="4"/>
+    </row>
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B177" s="4"/>
+      <c r="C177" s="4"/>
+    </row>
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B178" s="4"/>
+      <c r="C178" s="4"/>
+    </row>
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B179" s="4"/>
+      <c r="C179" s="4"/>
+    </row>
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B180" s="4"/>
+      <c r="C180" s="4"/>
+    </row>
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B181" s="4"/>
+      <c r="C181" s="4"/>
+    </row>
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B182" s="4"/>
+      <c r="C182" s="4"/>
+    </row>
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B183" s="4"/>
+      <c r="C183" s="4"/>
+    </row>
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B184" s="4"/>
+      <c r="C184" s="4"/>
+    </row>
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B185" s="4"/>
+      <c r="C185" s="4"/>
+    </row>
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B186" s="4"/>
+      <c r="C186" s="4"/>
+    </row>
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B187" s="4"/>
+      <c r="C187" s="4"/>
+    </row>
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B188" s="4"/>
+      <c r="C188" s="4"/>
+    </row>
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B189" s="4"/>
+      <c r="C189" s="4"/>
+    </row>
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B190" s="4"/>
+      <c r="C190" s="4"/>
+    </row>
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B191" s="4"/>
+      <c r="C191" s="4"/>
+    </row>
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B192" s="4"/>
+      <c r="C192" s="4"/>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B193" s="4"/>
+      <c r="C193" s="4"/>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B194" s="4"/>
+      <c r="C194" s="4"/>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B195" s="4"/>
+      <c r="C195" s="4"/>
+    </row>
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B196" s="4"/>
+      <c r="C196" s="4"/>
+    </row>
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B197" s="4"/>
+      <c r="C197" s="4"/>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B198" s="4"/>
+      <c r="C198" s="4"/>
+    </row>
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B199" s="4"/>
+      <c r="C199" s="4"/>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B200" s="4"/>
+      <c r="C200" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F75CE0-A1C1-4DE3-8C32-09CA7DE610E7}">
+  <dimension ref="A1:F197"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.75" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="9" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">

</xml_diff>